<commit_message>
feat: delete card '码A' and '码O'
</commit_message>
<xml_diff>
--- a/server/data/users.xlsx
+++ b/server/data/users.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wys/Code/lottery-ie/server/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A1AF2712-5B68-B04B-8435-D6E0AED231B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{725AC378-75A6-2D43-8518-F7FBB56BB00B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1400" yWindow="1320" windowWidth="27840" windowHeight="16620" xr2:uid="{9788348B-2A61-7548-ABA8-2AC16F6AF4CA}"/>
+    <workbookView xWindow="1400" yWindow="1320" windowWidth="27840" windowHeight="16620" xr2:uid="{F862E0E2-13A7-9941-92C1-EC7B5C489671}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="773">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="553">
   <si>
     <t>工号</t>
   </si>
@@ -1366,171 +1366,6 @@
     <t>码L55</t>
   </si>
   <si>
-    <t>码A01</t>
-  </si>
-  <si>
-    <t>码A02</t>
-  </si>
-  <si>
-    <t>码A03</t>
-  </si>
-  <si>
-    <t>码A04</t>
-  </si>
-  <si>
-    <t>码A05</t>
-  </si>
-  <si>
-    <t>码A06</t>
-  </si>
-  <si>
-    <t>码A07</t>
-  </si>
-  <si>
-    <t>码A08</t>
-  </si>
-  <si>
-    <t>码A09</t>
-  </si>
-  <si>
-    <t>码A10</t>
-  </si>
-  <si>
-    <t>码A11</t>
-  </si>
-  <si>
-    <t>码A12</t>
-  </si>
-  <si>
-    <t>码A13</t>
-  </si>
-  <si>
-    <t>码A14</t>
-  </si>
-  <si>
-    <t>码A15</t>
-  </si>
-  <si>
-    <t>码A16</t>
-  </si>
-  <si>
-    <t>码A17</t>
-  </si>
-  <si>
-    <t>码A18</t>
-  </si>
-  <si>
-    <t>码A19</t>
-  </si>
-  <si>
-    <t>码A20</t>
-  </si>
-  <si>
-    <t>码A21</t>
-  </si>
-  <si>
-    <t>码A22</t>
-  </si>
-  <si>
-    <t>码A23</t>
-  </si>
-  <si>
-    <t>码A24</t>
-  </si>
-  <si>
-    <t>码A25</t>
-  </si>
-  <si>
-    <t>码A26</t>
-  </si>
-  <si>
-    <t>码A27</t>
-  </si>
-  <si>
-    <t>码A28</t>
-  </si>
-  <si>
-    <t>码A29</t>
-  </si>
-  <si>
-    <t>码A30</t>
-  </si>
-  <si>
-    <t>码A31</t>
-  </si>
-  <si>
-    <t>码A32</t>
-  </si>
-  <si>
-    <t>码A33</t>
-  </si>
-  <si>
-    <t>码A34</t>
-  </si>
-  <si>
-    <t>码A35</t>
-  </si>
-  <si>
-    <t>码A36</t>
-  </si>
-  <si>
-    <t>码A37</t>
-  </si>
-  <si>
-    <t>码A38</t>
-  </si>
-  <si>
-    <t>码A39</t>
-  </si>
-  <si>
-    <t>码A40</t>
-  </si>
-  <si>
-    <t>码A41</t>
-  </si>
-  <si>
-    <t>码A42</t>
-  </si>
-  <si>
-    <t>码A43</t>
-  </si>
-  <si>
-    <t>码A44</t>
-  </si>
-  <si>
-    <t>码A45</t>
-  </si>
-  <si>
-    <t>码A46</t>
-  </si>
-  <si>
-    <t>码A47</t>
-  </si>
-  <si>
-    <t>码A48</t>
-  </si>
-  <si>
-    <t>码A49</t>
-  </si>
-  <si>
-    <t>码A50</t>
-  </si>
-  <si>
-    <t>码A51</t>
-  </si>
-  <si>
-    <t>码A52</t>
-  </si>
-  <si>
-    <t>码A53</t>
-  </si>
-  <si>
-    <t>码A54</t>
-  </si>
-  <si>
-    <t>码A55</t>
-  </si>
-  <si>
     <t>码W01</t>
   </si>
   <si>
@@ -1694,501 +1529,6 @@
   </si>
   <si>
     <t>码W55</t>
-  </si>
-  <si>
-    <t>码C01</t>
-  </si>
-  <si>
-    <t>码C02</t>
-  </si>
-  <si>
-    <t>码C03</t>
-  </si>
-  <si>
-    <t>码C04</t>
-  </si>
-  <si>
-    <t>码C05</t>
-  </si>
-  <si>
-    <t>码C06</t>
-  </si>
-  <si>
-    <t>码C07</t>
-  </si>
-  <si>
-    <t>码C08</t>
-  </si>
-  <si>
-    <t>码C09</t>
-  </si>
-  <si>
-    <t>码C10</t>
-  </si>
-  <si>
-    <t>码C11</t>
-  </si>
-  <si>
-    <t>码C12</t>
-  </si>
-  <si>
-    <t>码C13</t>
-  </si>
-  <si>
-    <t>码C14</t>
-  </si>
-  <si>
-    <t>码C15</t>
-  </si>
-  <si>
-    <t>码C16</t>
-  </si>
-  <si>
-    <t>码C17</t>
-  </si>
-  <si>
-    <t>码C18</t>
-  </si>
-  <si>
-    <t>码C19</t>
-  </si>
-  <si>
-    <t>码C20</t>
-  </si>
-  <si>
-    <t>码C21</t>
-  </si>
-  <si>
-    <t>码C22</t>
-  </si>
-  <si>
-    <t>码C23</t>
-  </si>
-  <si>
-    <t>码C24</t>
-  </si>
-  <si>
-    <t>码C25</t>
-  </si>
-  <si>
-    <t>码C26</t>
-  </si>
-  <si>
-    <t>码C27</t>
-  </si>
-  <si>
-    <t>码C28</t>
-  </si>
-  <si>
-    <t>码C29</t>
-  </si>
-  <si>
-    <t>码C30</t>
-  </si>
-  <si>
-    <t>码C31</t>
-  </si>
-  <si>
-    <t>码C32</t>
-  </si>
-  <si>
-    <t>码C33</t>
-  </si>
-  <si>
-    <t>码C34</t>
-  </si>
-  <si>
-    <t>码C35</t>
-  </si>
-  <si>
-    <t>码C36</t>
-  </si>
-  <si>
-    <t>码C37</t>
-  </si>
-  <si>
-    <t>码C38</t>
-  </si>
-  <si>
-    <t>码C39</t>
-  </si>
-  <si>
-    <t>码C40</t>
-  </si>
-  <si>
-    <t>码C41</t>
-  </si>
-  <si>
-    <t>码C42</t>
-  </si>
-  <si>
-    <t>码C43</t>
-  </si>
-  <si>
-    <t>码C44</t>
-  </si>
-  <si>
-    <t>码C45</t>
-  </si>
-  <si>
-    <t>码C46</t>
-  </si>
-  <si>
-    <t>码C47</t>
-  </si>
-  <si>
-    <t>码C48</t>
-  </si>
-  <si>
-    <t>码C49</t>
-  </si>
-  <si>
-    <t>码C50</t>
-  </si>
-  <si>
-    <t>码C51</t>
-  </si>
-  <si>
-    <t>码C52</t>
-  </si>
-  <si>
-    <t>码C53</t>
-  </si>
-  <si>
-    <t>码C54</t>
-  </si>
-  <si>
-    <t>码C55</t>
-  </si>
-  <si>
-    <t>码O01</t>
-  </si>
-  <si>
-    <t>码O02</t>
-  </si>
-  <si>
-    <t>码O03</t>
-  </si>
-  <si>
-    <t>码O04</t>
-  </si>
-  <si>
-    <t>码O05</t>
-  </si>
-  <si>
-    <t>码O06</t>
-  </si>
-  <si>
-    <t>码O07</t>
-  </si>
-  <si>
-    <t>码O08</t>
-  </si>
-  <si>
-    <t>码O09</t>
-  </si>
-  <si>
-    <t>码O10</t>
-  </si>
-  <si>
-    <t>码O11</t>
-  </si>
-  <si>
-    <t>码O12</t>
-  </si>
-  <si>
-    <t>码O13</t>
-  </si>
-  <si>
-    <t>码O14</t>
-  </si>
-  <si>
-    <t>码O15</t>
-  </si>
-  <si>
-    <t>码O16</t>
-  </si>
-  <si>
-    <t>码O17</t>
-  </si>
-  <si>
-    <t>码O18</t>
-  </si>
-  <si>
-    <t>码O19</t>
-  </si>
-  <si>
-    <t>码O20</t>
-  </si>
-  <si>
-    <t>码O21</t>
-  </si>
-  <si>
-    <t>码O22</t>
-  </si>
-  <si>
-    <t>码O23</t>
-  </si>
-  <si>
-    <t>码O24</t>
-  </si>
-  <si>
-    <t>码O25</t>
-  </si>
-  <si>
-    <t>码O26</t>
-  </si>
-  <si>
-    <t>码O27</t>
-  </si>
-  <si>
-    <t>码O28</t>
-  </si>
-  <si>
-    <t>码O29</t>
-  </si>
-  <si>
-    <t>码O30</t>
-  </si>
-  <si>
-    <t>码O31</t>
-  </si>
-  <si>
-    <t>码O32</t>
-  </si>
-  <si>
-    <t>码O33</t>
-  </si>
-  <si>
-    <t>码O34</t>
-  </si>
-  <si>
-    <t>码O35</t>
-  </si>
-  <si>
-    <t>码O36</t>
-  </si>
-  <si>
-    <t>码O37</t>
-  </si>
-  <si>
-    <t>码O38</t>
-  </si>
-  <si>
-    <t>码O39</t>
-  </si>
-  <si>
-    <t>码O40</t>
-  </si>
-  <si>
-    <t>码O41</t>
-  </si>
-  <si>
-    <t>码O42</t>
-  </si>
-  <si>
-    <t>码O43</t>
-  </si>
-  <si>
-    <t>码O44</t>
-  </si>
-  <si>
-    <t>码O45</t>
-  </si>
-  <si>
-    <t>码O46</t>
-  </si>
-  <si>
-    <t>码O47</t>
-  </si>
-  <si>
-    <t>码O48</t>
-  </si>
-  <si>
-    <t>码O49</t>
-  </si>
-  <si>
-    <t>码O50</t>
-  </si>
-  <si>
-    <t>码O51</t>
-  </si>
-  <si>
-    <t>码O52</t>
-  </si>
-  <si>
-    <t>码O53</t>
-  </si>
-  <si>
-    <t>码O54</t>
-  </si>
-  <si>
-    <t>码O55</t>
-  </si>
-  <si>
-    <t>码D01</t>
-  </si>
-  <si>
-    <t>码D02</t>
-  </si>
-  <si>
-    <t>码D03</t>
-  </si>
-  <si>
-    <t>码D04</t>
-  </si>
-  <si>
-    <t>码D05</t>
-  </si>
-  <si>
-    <t>码D06</t>
-  </si>
-  <si>
-    <t>码D07</t>
-  </si>
-  <si>
-    <t>码D08</t>
-  </si>
-  <si>
-    <t>码D09</t>
-  </si>
-  <si>
-    <t>码D10</t>
-  </si>
-  <si>
-    <t>码D11</t>
-  </si>
-  <si>
-    <t>码D12</t>
-  </si>
-  <si>
-    <t>码D13</t>
-  </si>
-  <si>
-    <t>码D14</t>
-  </si>
-  <si>
-    <t>码D15</t>
-  </si>
-  <si>
-    <t>码D16</t>
-  </si>
-  <si>
-    <t>码D17</t>
-  </si>
-  <si>
-    <t>码D18</t>
-  </si>
-  <si>
-    <t>码D19</t>
-  </si>
-  <si>
-    <t>码D20</t>
-  </si>
-  <si>
-    <t>码D21</t>
-  </si>
-  <si>
-    <t>码D22</t>
-  </si>
-  <si>
-    <t>码D23</t>
-  </si>
-  <si>
-    <t>码D24</t>
-  </si>
-  <si>
-    <t>码D25</t>
-  </si>
-  <si>
-    <t>码D26</t>
-  </si>
-  <si>
-    <t>码D27</t>
-  </si>
-  <si>
-    <t>码D28</t>
-  </si>
-  <si>
-    <t>码D29</t>
-  </si>
-  <si>
-    <t>码D30</t>
-  </si>
-  <si>
-    <t>码D31</t>
-  </si>
-  <si>
-    <t>码D32</t>
-  </si>
-  <si>
-    <t>码D33</t>
-  </si>
-  <si>
-    <t>码D34</t>
-  </si>
-  <si>
-    <t>码D35</t>
-  </si>
-  <si>
-    <t>码D36</t>
-  </si>
-  <si>
-    <t>码D37</t>
-  </si>
-  <si>
-    <t>码D38</t>
-  </si>
-  <si>
-    <t>码D39</t>
-  </si>
-  <si>
-    <t>码D40</t>
-  </si>
-  <si>
-    <t>码D41</t>
-  </si>
-  <si>
-    <t>码D42</t>
-  </si>
-  <si>
-    <t>码D43</t>
-  </si>
-  <si>
-    <t>码D44</t>
-  </si>
-  <si>
-    <t>码D45</t>
-  </si>
-  <si>
-    <t>码D46</t>
-  </si>
-  <si>
-    <t>码D47</t>
-  </si>
-  <si>
-    <t>码D48</t>
-  </si>
-  <si>
-    <t>码D49</t>
-  </si>
-  <si>
-    <t>码D50</t>
-  </si>
-  <si>
-    <t>码D51</t>
-  </si>
-  <si>
-    <t>码D52</t>
-  </si>
-  <si>
-    <t>码D53</t>
-  </si>
-  <si>
-    <t>码D54</t>
-  </si>
-  <si>
-    <t>码D55</t>
   </si>
   <si>
     <t>码E01</t>
@@ -2716,11 +2056,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37992013-7309-3740-BA51-458600DDCA72}">
-  <dimension ref="A1:C771"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E42194F-AC21-C147-BB74-93705BFB8F4D}">
+  <dimension ref="A1:C551"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A276" workbookViewId="0">
-      <selection activeCell="H284" sqref="H284"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C551"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5486,1106 +4826,6 @@
         <v>552</v>
       </c>
     </row>
-    <row r="552" spans="2:2">
-      <c r="B552" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="553" spans="2:2">
-      <c r="B553" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="554" spans="2:2">
-      <c r="B554" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="555" spans="2:2">
-      <c r="B555" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="556" spans="2:2">
-      <c r="B556" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="557" spans="2:2">
-      <c r="B557" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="558" spans="2:2">
-      <c r="B558" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="559" spans="2:2">
-      <c r="B559" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="560" spans="2:2">
-      <c r="B560" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="561" spans="2:2">
-      <c r="B561" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="562" spans="2:2">
-      <c r="B562" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="563" spans="2:2">
-      <c r="B563" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="564" spans="2:2">
-      <c r="B564" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="565" spans="2:2">
-      <c r="B565" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="566" spans="2:2">
-      <c r="B566" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="567" spans="2:2">
-      <c r="B567" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="568" spans="2:2">
-      <c r="B568" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="569" spans="2:2">
-      <c r="B569" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="570" spans="2:2">
-      <c r="B570" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="571" spans="2:2">
-      <c r="B571" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="572" spans="2:2">
-      <c r="B572" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="573" spans="2:2">
-      <c r="B573" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="574" spans="2:2">
-      <c r="B574" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="575" spans="2:2">
-      <c r="B575" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="576" spans="2:2">
-      <c r="B576" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="577" spans="2:2">
-      <c r="B577" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="578" spans="2:2">
-      <c r="B578" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="579" spans="2:2">
-      <c r="B579" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="580" spans="2:2">
-      <c r="B580" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="581" spans="2:2">
-      <c r="B581" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="582" spans="2:2">
-      <c r="B582" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="583" spans="2:2">
-      <c r="B583" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="584" spans="2:2">
-      <c r="B584" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="585" spans="2:2">
-      <c r="B585" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="586" spans="2:2">
-      <c r="B586" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="587" spans="2:2">
-      <c r="B587" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="588" spans="2:2">
-      <c r="B588" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="589" spans="2:2">
-      <c r="B589" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="590" spans="2:2">
-      <c r="B590" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="591" spans="2:2">
-      <c r="B591" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="592" spans="2:2">
-      <c r="B592" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="593" spans="2:2">
-      <c r="B593" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="594" spans="2:2">
-      <c r="B594" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="595" spans="2:2">
-      <c r="B595" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="596" spans="2:2">
-      <c r="B596" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="597" spans="2:2">
-      <c r="B597" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="598" spans="2:2">
-      <c r="B598" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="599" spans="2:2">
-      <c r="B599" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="600" spans="2:2">
-      <c r="B600" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="601" spans="2:2">
-      <c r="B601" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="602" spans="2:2">
-      <c r="B602" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="603" spans="2:2">
-      <c r="B603" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="604" spans="2:2">
-      <c r="B604" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="605" spans="2:2">
-      <c r="B605" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="606" spans="2:2">
-      <c r="B606" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="607" spans="2:2">
-      <c r="B607" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="608" spans="2:2">
-      <c r="B608" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="609" spans="2:2">
-      <c r="B609" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="610" spans="2:2">
-      <c r="B610" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="611" spans="2:2">
-      <c r="B611" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="612" spans="2:2">
-      <c r="B612" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="613" spans="2:2">
-      <c r="B613" t="s">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="614" spans="2:2">
-      <c r="B614" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="615" spans="2:2">
-      <c r="B615" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="616" spans="2:2">
-      <c r="B616" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="617" spans="2:2">
-      <c r="B617" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="618" spans="2:2">
-      <c r="B618" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="619" spans="2:2">
-      <c r="B619" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="620" spans="2:2">
-      <c r="B620" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="621" spans="2:2">
-      <c r="B621" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="622" spans="2:2">
-      <c r="B622" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="623" spans="2:2">
-      <c r="B623" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="624" spans="2:2">
-      <c r="B624" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="625" spans="2:2">
-      <c r="B625" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="626" spans="2:2">
-      <c r="B626" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="627" spans="2:2">
-      <c r="B627" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="628" spans="2:2">
-      <c r="B628" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="629" spans="2:2">
-      <c r="B629" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="630" spans="2:2">
-      <c r="B630" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="631" spans="2:2">
-      <c r="B631" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="632" spans="2:2">
-      <c r="B632" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="633" spans="2:2">
-      <c r="B633" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="634" spans="2:2">
-      <c r="B634" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="635" spans="2:2">
-      <c r="B635" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="636" spans="2:2">
-      <c r="B636" t="s">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="637" spans="2:2">
-      <c r="B637" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="638" spans="2:2">
-      <c r="B638" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="639" spans="2:2">
-      <c r="B639" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="640" spans="2:2">
-      <c r="B640" t="s">
-        <v>641</v>
-      </c>
-    </row>
-    <row r="641" spans="2:2">
-      <c r="B641" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="642" spans="2:2">
-      <c r="B642" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="643" spans="2:2">
-      <c r="B643" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="644" spans="2:2">
-      <c r="B644" t="s">
-        <v>645</v>
-      </c>
-    </row>
-    <row r="645" spans="2:2">
-      <c r="B645" t="s">
-        <v>646</v>
-      </c>
-    </row>
-    <row r="646" spans="2:2">
-      <c r="B646" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="647" spans="2:2">
-      <c r="B647" t="s">
-        <v>648</v>
-      </c>
-    </row>
-    <row r="648" spans="2:2">
-      <c r="B648" t="s">
-        <v>649</v>
-      </c>
-    </row>
-    <row r="649" spans="2:2">
-      <c r="B649" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="650" spans="2:2">
-      <c r="B650" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="651" spans="2:2">
-      <c r="B651" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="652" spans="2:2">
-      <c r="B652" t="s">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="653" spans="2:2">
-      <c r="B653" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="654" spans="2:2">
-      <c r="B654" t="s">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="655" spans="2:2">
-      <c r="B655" t="s">
-        <v>656</v>
-      </c>
-    </row>
-    <row r="656" spans="2:2">
-      <c r="B656" t="s">
-        <v>657</v>
-      </c>
-    </row>
-    <row r="657" spans="2:2">
-      <c r="B657" t="s">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="658" spans="2:2">
-      <c r="B658" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="659" spans="2:2">
-      <c r="B659" t="s">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="660" spans="2:2">
-      <c r="B660" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="661" spans="2:2">
-      <c r="B661" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="662" spans="2:2">
-      <c r="B662" t="s">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="663" spans="2:2">
-      <c r="B663" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="664" spans="2:2">
-      <c r="B664" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="665" spans="2:2">
-      <c r="B665" t="s">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="666" spans="2:2">
-      <c r="B666" t="s">
-        <v>667</v>
-      </c>
-    </row>
-    <row r="667" spans="2:2">
-      <c r="B667" t="s">
-        <v>668</v>
-      </c>
-    </row>
-    <row r="668" spans="2:2">
-      <c r="B668" t="s">
-        <v>669</v>
-      </c>
-    </row>
-    <row r="669" spans="2:2">
-      <c r="B669" t="s">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="670" spans="2:2">
-      <c r="B670" t="s">
-        <v>671</v>
-      </c>
-    </row>
-    <row r="671" spans="2:2">
-      <c r="B671" t="s">
-        <v>672</v>
-      </c>
-    </row>
-    <row r="672" spans="2:2">
-      <c r="B672" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="673" spans="2:2">
-      <c r="B673" t="s">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="674" spans="2:2">
-      <c r="B674" t="s">
-        <v>675</v>
-      </c>
-    </row>
-    <row r="675" spans="2:2">
-      <c r="B675" t="s">
-        <v>676</v>
-      </c>
-    </row>
-    <row r="676" spans="2:2">
-      <c r="B676" t="s">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="677" spans="2:2">
-      <c r="B677" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="678" spans="2:2">
-      <c r="B678" t="s">
-        <v>679</v>
-      </c>
-    </row>
-    <row r="679" spans="2:2">
-      <c r="B679" t="s">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="680" spans="2:2">
-      <c r="B680" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="681" spans="2:2">
-      <c r="B681" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="682" spans="2:2">
-      <c r="B682" t="s">
-        <v>683</v>
-      </c>
-    </row>
-    <row r="683" spans="2:2">
-      <c r="B683" t="s">
-        <v>684</v>
-      </c>
-    </row>
-    <row r="684" spans="2:2">
-      <c r="B684" t="s">
-        <v>685</v>
-      </c>
-    </row>
-    <row r="685" spans="2:2">
-      <c r="B685" t="s">
-        <v>686</v>
-      </c>
-    </row>
-    <row r="686" spans="2:2">
-      <c r="B686" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="687" spans="2:2">
-      <c r="B687" t="s">
-        <v>688</v>
-      </c>
-    </row>
-    <row r="688" spans="2:2">
-      <c r="B688" t="s">
-        <v>689</v>
-      </c>
-    </row>
-    <row r="689" spans="2:2">
-      <c r="B689" t="s">
-        <v>690</v>
-      </c>
-    </row>
-    <row r="690" spans="2:2">
-      <c r="B690" t="s">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="691" spans="2:2">
-      <c r="B691" t="s">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="692" spans="2:2">
-      <c r="B692" t="s">
-        <v>693</v>
-      </c>
-    </row>
-    <row r="693" spans="2:2">
-      <c r="B693" t="s">
-        <v>694</v>
-      </c>
-    </row>
-    <row r="694" spans="2:2">
-      <c r="B694" t="s">
-        <v>695</v>
-      </c>
-    </row>
-    <row r="695" spans="2:2">
-      <c r="B695" t="s">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="696" spans="2:2">
-      <c r="B696" t="s">
-        <v>697</v>
-      </c>
-    </row>
-    <row r="697" spans="2:2">
-      <c r="B697" t="s">
-        <v>698</v>
-      </c>
-    </row>
-    <row r="698" spans="2:2">
-      <c r="B698" t="s">
-        <v>699</v>
-      </c>
-    </row>
-    <row r="699" spans="2:2">
-      <c r="B699" t="s">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="700" spans="2:2">
-      <c r="B700" t="s">
-        <v>701</v>
-      </c>
-    </row>
-    <row r="701" spans="2:2">
-      <c r="B701" t="s">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="702" spans="2:2">
-      <c r="B702" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="703" spans="2:2">
-      <c r="B703" t="s">
-        <v>704</v>
-      </c>
-    </row>
-    <row r="704" spans="2:2">
-      <c r="B704" t="s">
-        <v>705</v>
-      </c>
-    </row>
-    <row r="705" spans="2:2">
-      <c r="B705" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="706" spans="2:2">
-      <c r="B706" t="s">
-        <v>707</v>
-      </c>
-    </row>
-    <row r="707" spans="2:2">
-      <c r="B707" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="708" spans="2:2">
-      <c r="B708" t="s">
-        <v>709</v>
-      </c>
-    </row>
-    <row r="709" spans="2:2">
-      <c r="B709" t="s">
-        <v>710</v>
-      </c>
-    </row>
-    <row r="710" spans="2:2">
-      <c r="B710" t="s">
-        <v>711</v>
-      </c>
-    </row>
-    <row r="711" spans="2:2">
-      <c r="B711" t="s">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="712" spans="2:2">
-      <c r="B712" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="713" spans="2:2">
-      <c r="B713" t="s">
-        <v>714</v>
-      </c>
-    </row>
-    <row r="714" spans="2:2">
-      <c r="B714" t="s">
-        <v>715</v>
-      </c>
-    </row>
-    <row r="715" spans="2:2">
-      <c r="B715" t="s">
-        <v>716</v>
-      </c>
-    </row>
-    <row r="716" spans="2:2">
-      <c r="B716" t="s">
-        <v>717</v>
-      </c>
-    </row>
-    <row r="717" spans="2:2">
-      <c r="B717" t="s">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="718" spans="2:2">
-      <c r="B718" t="s">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="719" spans="2:2">
-      <c r="B719" t="s">
-        <v>720</v>
-      </c>
-    </row>
-    <row r="720" spans="2:2">
-      <c r="B720" t="s">
-        <v>721</v>
-      </c>
-    </row>
-    <row r="721" spans="2:2">
-      <c r="B721" t="s">
-        <v>722</v>
-      </c>
-    </row>
-    <row r="722" spans="2:2">
-      <c r="B722" t="s">
-        <v>723</v>
-      </c>
-    </row>
-    <row r="723" spans="2:2">
-      <c r="B723" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="724" spans="2:2">
-      <c r="B724" t="s">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="725" spans="2:2">
-      <c r="B725" t="s">
-        <v>726</v>
-      </c>
-    </row>
-    <row r="726" spans="2:2">
-      <c r="B726" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="727" spans="2:2">
-      <c r="B727" t="s">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="728" spans="2:2">
-      <c r="B728" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="729" spans="2:2">
-      <c r="B729" t="s">
-        <v>730</v>
-      </c>
-    </row>
-    <row r="730" spans="2:2">
-      <c r="B730" t="s">
-        <v>731</v>
-      </c>
-    </row>
-    <row r="731" spans="2:2">
-      <c r="B731" t="s">
-        <v>732</v>
-      </c>
-    </row>
-    <row r="732" spans="2:2">
-      <c r="B732" t="s">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="733" spans="2:2">
-      <c r="B733" t="s">
-        <v>734</v>
-      </c>
-    </row>
-    <row r="734" spans="2:2">
-      <c r="B734" t="s">
-        <v>735</v>
-      </c>
-    </row>
-    <row r="735" spans="2:2">
-      <c r="B735" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row r="736" spans="2:2">
-      <c r="B736" t="s">
-        <v>737</v>
-      </c>
-    </row>
-    <row r="737" spans="2:2">
-      <c r="B737" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row r="738" spans="2:2">
-      <c r="B738" t="s">
-        <v>739</v>
-      </c>
-    </row>
-    <row r="739" spans="2:2">
-      <c r="B739" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="740" spans="2:2">
-      <c r="B740" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="741" spans="2:2">
-      <c r="B741" t="s">
-        <v>742</v>
-      </c>
-    </row>
-    <row r="742" spans="2:2">
-      <c r="B742" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="743" spans="2:2">
-      <c r="B743" t="s">
-        <v>744</v>
-      </c>
-    </row>
-    <row r="744" spans="2:2">
-      <c r="B744" t="s">
-        <v>745</v>
-      </c>
-    </row>
-    <row r="745" spans="2:2">
-      <c r="B745" t="s">
-        <v>746</v>
-      </c>
-    </row>
-    <row r="746" spans="2:2">
-      <c r="B746" t="s">
-        <v>747</v>
-      </c>
-    </row>
-    <row r="747" spans="2:2">
-      <c r="B747" t="s">
-        <v>748</v>
-      </c>
-    </row>
-    <row r="748" spans="2:2">
-      <c r="B748" t="s">
-        <v>749</v>
-      </c>
-    </row>
-    <row r="749" spans="2:2">
-      <c r="B749" t="s">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="750" spans="2:2">
-      <c r="B750" t="s">
-        <v>751</v>
-      </c>
-    </row>
-    <row r="751" spans="2:2">
-      <c r="B751" t="s">
-        <v>752</v>
-      </c>
-    </row>
-    <row r="752" spans="2:2">
-      <c r="B752" t="s">
-        <v>753</v>
-      </c>
-    </row>
-    <row r="753" spans="2:2">
-      <c r="B753" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="754" spans="2:2">
-      <c r="B754" t="s">
-        <v>755</v>
-      </c>
-    </row>
-    <row r="755" spans="2:2">
-      <c r="B755" t="s">
-        <v>756</v>
-      </c>
-    </row>
-    <row r="756" spans="2:2">
-      <c r="B756" t="s">
-        <v>757</v>
-      </c>
-    </row>
-    <row r="757" spans="2:2">
-      <c r="B757" t="s">
-        <v>758</v>
-      </c>
-    </row>
-    <row r="758" spans="2:2">
-      <c r="B758" t="s">
-        <v>759</v>
-      </c>
-    </row>
-    <row r="759" spans="2:2">
-      <c r="B759" t="s">
-        <v>760</v>
-      </c>
-    </row>
-    <row r="760" spans="2:2">
-      <c r="B760" t="s">
-        <v>761</v>
-      </c>
-    </row>
-    <row r="761" spans="2:2">
-      <c r="B761" t="s">
-        <v>762</v>
-      </c>
-    </row>
-    <row r="762" spans="2:2">
-      <c r="B762" t="s">
-        <v>763</v>
-      </c>
-    </row>
-    <row r="763" spans="2:2">
-      <c r="B763" t="s">
-        <v>764</v>
-      </c>
-    </row>
-    <row r="764" spans="2:2">
-      <c r="B764" t="s">
-        <v>765</v>
-      </c>
-    </row>
-    <row r="765" spans="2:2">
-      <c r="B765" t="s">
-        <v>766</v>
-      </c>
-    </row>
-    <row r="766" spans="2:2">
-      <c r="B766" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="767" spans="2:2">
-      <c r="B767" t="s">
-        <v>768</v>
-      </c>
-    </row>
-    <row r="768" spans="2:2">
-      <c r="B768" t="s">
-        <v>769</v>
-      </c>
-    </row>
-    <row r="769" spans="2:2">
-      <c r="B769" t="s">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="770" spans="2:2">
-      <c r="B770" t="s">
-        <v>771</v>
-      </c>
-    </row>
-    <row r="771" spans="2:2">
-      <c r="B771" t="s">
-        <v>772</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>